<commit_message>
added use case distribution to the repo descriptive statistics
</commit_message>
<xml_diff>
--- a/data/577 Projects/ModelDataLoad.xlsx
+++ b/data/577 Projects/ModelDataLoad.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COCOMODataLoad" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="147">
   <si>
     <t>Team. NO.</t>
   </si>
@@ -437,6 +437,30 @@
   </si>
   <si>
     <t>s16b_Picshare_RA</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>F14a_soccer_data_web_crawler</t>
+  </si>
+  <si>
+    <t>Mobile Game</t>
+  </si>
+  <si>
+    <t>Mobile App</t>
+  </si>
+  <si>
+    <t>Web App</t>
+  </si>
+  <si>
+    <t>Desktop App</t>
+  </si>
+  <si>
+    <t>Mobile&amp;Web App</t>
+  </si>
+  <si>
+    <t>web App</t>
   </si>
 </sst>
 </file>
@@ -1273,21 +1297,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="56.85546875" customWidth="1"/>
-    <col min="4" max="8" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1298,88 +1323,91 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>58</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1389,80 +1417,80 @@
       <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="1">
         <v>3113</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>8271</v>
-      </c>
-      <c r="F2" s="1">
-        <v>8059</v>
       </c>
       <c r="G2" s="1">
         <v>8059</v>
       </c>
       <c r="H2" s="1">
-        <f>0.001*G2</f>
+        <v>8059</v>
+      </c>
+      <c r="I2" s="1">
+        <f>0.001*H2</f>
         <v>8.0590000000000011</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="X2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB2" s="3" t="s">
+      <c r="Z2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AC2" s="3" t="s">
@@ -1471,8 +1499,11 @@
       <c r="AD2" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="AE2" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1482,80 +1513,80 @@
       <c r="C3" t="s">
         <v>137</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3">
         <v>1592</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>8561</v>
-      </c>
-      <c r="F3">
-        <v>8209</v>
       </c>
       <c r="G3">
         <v>8209</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H26" si="0">0.001*G3</f>
+        <v>8209</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I26" si="0">0.001*H3</f>
         <v>8.2089999999999996</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
         <v>28</v>
       </c>
-      <c r="M3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" t="s">
         <v>29</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" t="s">
         <v>29</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W3" t="s">
         <v>27</v>
       </c>
       <c r="X3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y3" t="s">
         <v>28</v>
       </c>
-      <c r="Y3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB3" s="2" t="s">
+      <c r="Z3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB3" t="s">
         <v>29</v>
       </c>
       <c r="AC3" s="2" t="s">
@@ -1564,8 +1595,11 @@
       <c r="AD3" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="AE3" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1575,90 +1609,93 @@
       <c r="C4" t="s">
         <v>59</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4">
         <v>1142</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>10663</v>
-      </c>
-      <c r="F4">
-        <v>8100</v>
       </c>
       <c r="G4">
         <v>8100</v>
       </c>
       <c r="H4">
+        <v>8100</v>
+      </c>
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L4" t="s">
-        <v>27</v>
+      <c r="L4" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="Q4" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="2" t="s">
+      <c r="R4" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" t="s">
         <v>29</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V4" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W4" t="s">
         <v>29</v>
       </c>
       <c r="X4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Y4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB4" t="s">
         <v>29</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AD4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1668,90 +1705,93 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5">
         <v>1281</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>7593</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>56</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>7593</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>7.593</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
         <v>29</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="Q5" t="s">
-        <v>27</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" t="s">
         <v>29</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="W5" t="s">
         <v>29</v>
       </c>
       <c r="X5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Y5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB5" t="s">
         <v>32</v>
       </c>
-      <c r="AB5" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="AC5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="AD5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE5" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1761,90 +1801,93 @@
       <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6">
         <v>1347</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3679</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3257</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>3679</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f t="shared" si="0"/>
         <v>3.6790000000000003</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="M6" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="2" t="s">
         <v>29</v>
       </c>
       <c r="Q6" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T6" s="2" t="s">
+      <c r="S6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" t="s">
         <v>29</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V6" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W6" t="s">
         <v>27</v>
       </c>
       <c r="X6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y6" t="s">
         <v>28</v>
       </c>
-      <c r="Y6" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB6" s="2" t="s">
+      <c r="Z6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AD6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AD6" s="2" t="s">
+      <c r="AE6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1854,90 +1897,93 @@
       <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="1">
         <v>1482.5</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1386</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1045</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1386</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f t="shared" si="0"/>
         <v>1.3860000000000001</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="M7" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" t="s">
         <v>29</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="Q7" t="s">
         <v>29</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T7" s="2" t="s">
+      <c r="R7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T7" t="s">
         <v>29</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V7" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="X7" t="s">
         <v>27</v>
       </c>
       <c r="Y7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>27</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AD7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1947,62 +1993,62 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8">
         <v>617</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>5129</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>56</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>5129</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="0"/>
         <v>5.1290000000000004</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="J8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>26</v>
+        <v>26</v>
+      </c>
+      <c r="N8" t="s">
+        <v>29</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="Q8" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S8" t="s">
-        <v>29</v>
-      </c>
-      <c r="T8" s="2" t="s">
+      <c r="R8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T8" t="s">
         <v>29</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="W8" t="s">
@@ -2012,25 +2058,28 @@
         <v>29</v>
       </c>
       <c r="Y8" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB8" t="s">
         <v>26</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AD8" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="AE8" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2038,92 +2087,95 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9">
+        <v>140</v>
+      </c>
+      <c r="D9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9">
         <v>268.5</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>2258</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2000</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>2258</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="0"/>
         <v>2.258</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="P9" s="2" t="s">
         <v>27</v>
       </c>
       <c r="Q9" t="s">
         <v>27</v>
       </c>
-      <c r="R9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T9" s="2" t="s">
+      <c r="R9" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" t="s">
         <v>29</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V9" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y9" t="s">
         <v>28</v>
       </c>
-      <c r="Y9" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>26</v>
+      <c r="Z9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>29</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AD9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2133,90 +2185,93 @@
       <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10">
         <v>103</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2218</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>2000</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>2218</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f t="shared" si="0"/>
         <v>2.218</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>27</v>
       </c>
       <c r="M10" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" t="s">
         <v>29</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="Q10" t="s">
         <v>29</v>
       </c>
-      <c r="R10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S10" t="s">
-        <v>29</v>
-      </c>
-      <c r="T10" s="2" t="s">
+      <c r="R10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" t="s">
         <v>29</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V10" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="X10" t="s">
         <v>27</v>
       </c>
       <c r="Y10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB10" t="s">
         <v>32</v>
       </c>
-      <c r="AB10" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="AC10" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AD10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -2226,90 +2281,93 @@
       <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11">
         <v>146.5</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>9202</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>56</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>9202</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f t="shared" si="0"/>
         <v>9.202</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" t="s">
         <v>28</v>
       </c>
-      <c r="M11" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>27</v>
+      <c r="N11" t="s">
+        <v>29</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P11" t="s">
-        <v>29</v>
+      <c r="P11" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="Q11" t="s">
-        <v>26</v>
-      </c>
-      <c r="R11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S11" t="s">
-        <v>29</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="R11" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T11" t="s">
+        <v>29</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V11" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X11" t="s">
         <v>26</v>
       </c>
       <c r="Y11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>26</v>
       </c>
       <c r="AC11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AE11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2319,90 +2377,93 @@
       <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12">
         <v>125</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>7272</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>57</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1100</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J12" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="M12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" t="s">
         <v>27</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="Q12" t="s">
-        <v>27</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S12" t="s">
-        <v>29</v>
-      </c>
-      <c r="T12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T12" t="s">
         <v>29</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V12" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W12" t="s">
         <v>29</v>
       </c>
       <c r="X12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y12" t="s">
         <v>28</v>
       </c>
-      <c r="Y12" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB12" s="2" t="s">
-        <v>29</v>
+      <c r="Z12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>26</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AD12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE12" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2410,92 +2471,95 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13">
         <v>266</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>8779</v>
-      </c>
-      <c r="F13">
-        <v>730</v>
       </c>
       <c r="G13">
         <v>730</v>
       </c>
       <c r="H13">
+        <v>730</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="0"/>
         <v>0.73</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J13" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="M13" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>26</v>
+      <c r="N13" t="s">
+        <v>29</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="Q13" t="s">
         <v>26</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S13" t="s">
-        <v>29</v>
-      </c>
-      <c r="T13" s="2" t="s">
+      <c r="R13" t="s">
+        <v>26</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T13" t="s">
         <v>29</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V13" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W13" t="s">
         <v>29</v>
       </c>
       <c r="X13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y13" t="s">
         <v>28</v>
       </c>
-      <c r="Y13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB13" s="2" t="s">
-        <v>26</v>
+      <c r="Z13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>27</v>
       </c>
       <c r="AC13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AE13" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -2505,90 +2569,93 @@
       <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14">
         <v>571</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>9980</v>
-      </c>
-      <c r="F14">
-        <v>8116</v>
       </c>
       <c r="G14">
         <v>8116</v>
       </c>
       <c r="H14">
+        <v>8116</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="0"/>
         <v>8.1159999999999997</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="M14" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" t="s">
         <v>29</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="Q14" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S14" t="s">
-        <v>29</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="R14" t="s">
+        <v>29</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T14" t="s">
+        <v>29</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V14" t="s">
+        <v>27</v>
+      </c>
+      <c r="V14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="W14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="X14" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y14" t="s">
         <v>28</v>
       </c>
-      <c r="Y14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB14" s="2" t="s">
+      <c r="Z14" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB14" t="s">
         <v>29</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AD14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE14" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2598,90 +2665,93 @@
       <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15">
         <v>257.5</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F15">
-        <v>1500</v>
       </c>
       <c r="G15">
         <v>1500</v>
       </c>
       <c r="H15">
+        <v>1500</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="M15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" t="s">
         <v>29</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" t="s">
+        <v>29</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="Q15" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S15" t="s">
-        <v>29</v>
-      </c>
-      <c r="T15" s="2" t="s">
+      <c r="R15" t="s">
+        <v>26</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T15" t="s">
         <v>29</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V15" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W15" t="s">
         <v>28</v>
       </c>
       <c r="X15" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y15" t="s">
         <v>32</v>
       </c>
-      <c r="Y15" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB15" s="2" t="s">
+      <c r="Z15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB15" t="s">
         <v>27</v>
       </c>
       <c r="AC15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD15" s="2" t="s">
+      <c r="AE15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2691,90 +2761,93 @@
       <c r="C16" t="s">
         <v>42</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16">
         <v>140.5</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F16">
-        <v>3200</v>
       </c>
       <c r="G16">
         <v>3200</v>
       </c>
       <c r="H16">
+        <v>3200</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="J16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="M16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="N16" t="s">
+        <v>26</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="Q16" t="s">
-        <v>26</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S16" t="s">
-        <v>29</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="R16" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T16" t="s">
+        <v>29</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V16" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W16" t="s">
         <v>27</v>
       </c>
       <c r="X16" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y16" t="s">
         <v>28</v>
       </c>
-      <c r="Y16" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB16" s="2" t="s">
-        <v>27</v>
+      <c r="Z16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>29</v>
       </c>
       <c r="AC16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AE16" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2784,90 +2857,93 @@
       <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17">
         <v>482</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>6569</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>3200</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>6569</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="0"/>
         <v>6.569</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L17" t="s">
-        <v>27</v>
+      <c r="L17" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="M17" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="Q17" t="s">
-        <v>26</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S17" t="s">
-        <v>29</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="R17" t="s">
+        <v>26</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T17" t="s">
+        <v>29</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V17" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W17" t="s">
         <v>29</v>
       </c>
       <c r="X17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y17" t="s">
         <v>32</v>
       </c>
-      <c r="Y17" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB17" s="2" t="s">
+      <c r="Z17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB17" t="s">
         <v>29</v>
       </c>
       <c r="AC17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AE17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2877,90 +2953,93 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E18" s="1">
         <v>1965</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>7067</v>
-      </c>
-      <c r="F18">
-        <v>6415</v>
       </c>
       <c r="G18">
         <v>6415</v>
       </c>
       <c r="H18">
+        <v>6415</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="0"/>
         <v>6.415</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="M18" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" t="s">
         <v>29</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P18" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="Q18" t="s">
         <v>29</v>
       </c>
-      <c r="R18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S18" t="s">
-        <v>29</v>
-      </c>
-      <c r="T18" s="2" t="s">
+      <c r="R18" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T18" t="s">
         <v>29</v>
       </c>
       <c r="U18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V18" t="s">
-        <v>27</v>
+      <c r="V18" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="W18" t="s">
         <v>27</v>
       </c>
       <c r="X18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y18" t="s">
         <v>28</v>
       </c>
-      <c r="Y18" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>29</v>
+      <c r="Z18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>27</v>
       </c>
       <c r="AC18" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AD18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE18" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -2970,66 +3049,66 @@
       <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E19" s="1">
         <v>759</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>12651</v>
-      </c>
-      <c r="F19" s="1">
-        <v>12263</v>
       </c>
       <c r="G19" s="1">
         <v>12263</v>
       </c>
       <c r="H19" s="1">
+        <v>12263</v>
+      </c>
+      <c r="I19" s="1">
         <f t="shared" si="0"/>
         <v>12.263</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="J19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>27</v>
+      <c r="L19" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="U19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="X19" s="1" t="s">
         <v>27</v>
@@ -3037,23 +3116,26 @@
       <c r="Y19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Z19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB19" s="3" t="s">
-        <v>27</v>
+      <c r="Z19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="AC19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD19" s="3" t="s">
+      <c r="AE19" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -3063,90 +3145,93 @@
       <c r="C20" t="s">
         <v>48</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20">
         <v>804.5</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>7365</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>8720</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>7365</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <f t="shared" si="0"/>
         <v>7.3650000000000002</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="J20" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L20" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" t="s">
         <v>28</v>
       </c>
-      <c r="M20" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>27</v>
+      <c r="N20" t="s">
+        <v>29</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P20" t="s">
-        <v>29</v>
+      <c r="P20" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="Q20" t="s">
-        <v>26</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S20" t="s">
-        <v>29</v>
-      </c>
-      <c r="T20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" t="s">
+        <v>26</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T20" t="s">
         <v>29</v>
       </c>
       <c r="U20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V20" t="s">
+      <c r="V20" s="2" t="s">
         <v>29</v>
       </c>
       <c r="W20" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="X20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y20" t="s">
         <v>28</v>
       </c>
-      <c r="Y20" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z20" s="2" t="s">
+      <c r="Z20" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA20" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB20" s="2" t="s">
-        <v>29</v>
+      <c r="AB20" t="s">
+        <v>26</v>
       </c>
       <c r="AC20" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AD20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE20" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -3156,90 +3241,93 @@
       <c r="C21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" s="1">
         <v>263</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>7250</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>312288</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>7250</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <f t="shared" si="0"/>
         <v>7.25</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="J21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" s="1" t="s">
+      <c r="L21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N21" s="3" t="s">
+      <c r="N21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="Q21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T21" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="U21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V21" s="3" t="s">
         <v>27</v>
       </c>
       <c r="W21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="X21" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="Y21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Z21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB21" s="3" t="s">
+      <c r="Z21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AC21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="AD21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE21" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -3249,90 +3337,93 @@
       <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E22">
         <v>724</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>2671</v>
-      </c>
-      <c r="F22">
-        <v>2950</v>
       </c>
       <c r="G22">
         <v>2950</v>
       </c>
       <c r="H22">
+        <v>2950</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="0"/>
         <v>2.95</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="M22" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" t="s">
         <v>29</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P22" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="Q22" t="s">
-        <v>26</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S22" t="s">
-        <v>29</v>
-      </c>
-      <c r="T22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R22" t="s">
+        <v>26</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T22" t="s">
         <v>29</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V22" t="s">
+        <v>29</v>
+      </c>
+      <c r="V22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="W22" t="s">
         <v>27</v>
       </c>
       <c r="X22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y22" t="s">
         <v>28</v>
       </c>
-      <c r="Y22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB22" s="2" t="s">
+      <c r="Z22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB22" t="s">
         <v>29</v>
       </c>
       <c r="AC22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD22" s="2" t="s">
+      <c r="AE22" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3342,63 +3433,63 @@
       <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23">
         <v>302.5</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>5552</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>10232</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>552</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f t="shared" si="0"/>
         <v>0.55200000000000005</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J23" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L23" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="M23" t="s">
-        <v>26</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="N23" t="s">
+        <v>26</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P23" t="s">
-        <v>29</v>
+        <v>29</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="Q23" t="s">
+        <v>29</v>
+      </c>
+      <c r="R23" t="s">
         <v>28</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S23" t="s">
-        <v>29</v>
-      </c>
-      <c r="T23" s="2" t="s">
+      <c r="S23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T23" t="s">
         <v>29</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="V23" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="W23" t="s">
         <v>27</v>
@@ -3407,25 +3498,28 @@
         <v>27</v>
       </c>
       <c r="Y23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AA23" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB23" s="2" t="s">
+      <c r="AB23" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AC23" s="2" t="s">
+      <c r="AD23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AD23" s="2" t="s">
+      <c r="AE23" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3435,54 +3529,54 @@
       <c r="C24" t="s">
         <v>135</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24">
         <v>3680</v>
-      </c>
-      <c r="E24" t="s">
-        <v>56</v>
       </c>
       <c r="F24" t="s">
         <v>56</v>
       </c>
-      <c r="G24">
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24">
         <v>21344</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <f t="shared" si="0"/>
         <v>21.344000000000001</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>29</v>
@@ -3491,19 +3585,19 @@
         <v>29</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Y24" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="Z24" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="AA24" s="2" t="s">
         <v>29</v>
@@ -3512,13 +3606,16 @@
         <v>29</v>
       </c>
       <c r="AC24" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AD24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE24" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3528,51 +3625,51 @@
       <c r="C25" t="s">
         <v>132</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25">
         <v>1392</v>
-      </c>
-      <c r="E25" t="s">
-        <v>56</v>
       </c>
       <c r="F25" t="s">
         <v>56</v>
       </c>
-      <c r="G25">
+      <c r="G25" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25">
         <v>4710</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <f t="shared" si="0"/>
         <v>4.71</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>27</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S25" s="2" t="s">
         <v>27</v>
@@ -3581,19 +3678,19 @@
         <v>27</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="V25" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Z25" s="2" t="s">
         <v>29</v>
@@ -3610,8 +3707,11 @@
       <c r="AD25" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="AE25" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3621,54 +3721,54 @@
       <c r="C26" t="s">
         <v>134</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="s">
+        <v>141</v>
+      </c>
+      <c r="E26">
         <v>737</v>
-      </c>
-      <c r="E26" t="s">
-        <v>56</v>
       </c>
       <c r="F26" t="s">
         <v>56</v>
       </c>
-      <c r="G26">
+      <c r="G26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26">
         <v>3120</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <f t="shared" si="0"/>
         <v>3.12</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="J26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="O26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="T26" s="2" t="s">
         <v>29</v>
@@ -3683,10 +3783,10 @@
         <v>29</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Z26" s="2" t="s">
         <v>29</v>
@@ -3701,6 +3801,9 @@
         <v>29</v>
       </c>
       <c r="AD26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE26" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3713,10 +3816,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C3"/>
+      <selection pane="bottomLeft" activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6321,7 +6424,7 @@
         <v>4</v>
       </c>
       <c r="V25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W25" s="2">
         <v>2</v>
@@ -6350,7 +6453,7 @@
       </c>
       <c r="AE25">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>1.2049999999999998</v>
       </c>
       <c r="AF25">
         <f>1*3+1*3+1*3+1*2+1*1</f>
@@ -6426,13 +6529,13 @@
         <v>5</v>
       </c>
       <c r="V26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="2">
         <v>2</v>
       </c>
       <c r="X26" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y26" s="2">
         <v>2</v>
@@ -6455,7 +6558,7 @@
       </c>
       <c r="AE26">
         <f t="shared" si="1"/>
-        <v>1.3099999999999998</v>
+        <v>1.2349999999999999</v>
       </c>
       <c r="AF26">
         <f>1*3</f>

</xml_diff>

<commit_message>
added the script for multiple linear regression for use case points weights. Started the experiments on weight calibration
</commit_message>
<xml_diff>
--- a/data/577 Projects/ModelDataLoad.xlsx
+++ b/data/577 Projects/ModelDataLoad.xlsx
@@ -3816,28 +3816,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="V25" sqref="V25"/>
+      <selection pane="bottomLeft" activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="17" width="3" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.42578125" customWidth="1"/>
+    <col min="23" max="23" width="4.7109375" customWidth="1"/>
     <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="29" width="3" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
about to finish the bayesian script
</commit_message>
<xml_diff>
--- a/data/577 Projects/ModelDataLoad.xlsx
+++ b/data/577 Projects/ModelDataLoad.xlsx
@@ -15,12 +15,12 @@
     <sheet name="COCOMODataLoad" sheetId="2" r:id="rId1"/>
     <sheet name="UseCaseDataLoad" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="150">
   <si>
     <t>Team. NO.</t>
   </si>
@@ -461,6 +461,15 @@
   </si>
   <si>
     <t>web App</t>
+  </si>
+  <si>
+    <t>Simple_Actor</t>
+  </si>
+  <si>
+    <t>Average_Actor</t>
+  </si>
+  <si>
+    <t>Complex_Actor</t>
   </si>
 </sst>
 </file>
@@ -3814,12 +3823,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG42"/>
+  <dimension ref="A1:AJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="X11" sqref="X11"/>
+      <selection pane="bottomLeft" activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3842,7 +3851,7 @@
     <col min="25" max="29" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3937,13 +3946,22 @@
         <v>107</v>
       </c>
       <c r="AF1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4040,15 +4058,24 @@
         <f t="shared" ref="AE2:AE26" si="1">1.4+(-0.03*(V2*$X$33+W2*$X$34+X2*$X$35+Y2*$X$36+Z2*$X$37+AA2*$X$38+AB2*$X$39+AC2*$X$40))</f>
         <v>1.0249999999999999</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI2">
         <f>1*3+1*3+1*2</f>
         <v>8</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AJ2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4145,15 +4172,24 @@
         <f t="shared" si="1"/>
         <v>0.87499999999999989</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
         <f>1*3+1*3</f>
         <v>6</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AJ3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4251,14 +4287,23 @@
         <v>0.85999999999999988</v>
       </c>
       <c r="AF4">
+        <v>2</v>
+      </c>
+      <c r="AG4">
+        <v>2</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
         <f>1*3+1*3</f>
         <v>6</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AJ4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4356,14 +4401,23 @@
         <v>0.91999999999999993</v>
       </c>
       <c r="AF5">
+        <v>3</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
         <f>1*3+1*3</f>
         <v>6</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AJ5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4461,14 +4515,23 @@
         <v>0.8899999999999999</v>
       </c>
       <c r="AF6">
+        <v>2</v>
+      </c>
+      <c r="AG6">
+        <v>2</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AJ6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4566,14 +4629,23 @@
         <v>0.95</v>
       </c>
       <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
         <f>1*3+1*3</f>
         <v>6</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AJ7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4671,14 +4743,23 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>3</v>
+      </c>
+      <c r="AH8">
+        <v>3</v>
+      </c>
+      <c r="AI8">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AJ8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -4776,14 +4857,23 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AF9">
+        <v>2</v>
+      </c>
+      <c r="AG9">
+        <v>2</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
         <f>1*3+1*3</f>
         <v>6</v>
       </c>
-      <c r="AG9" t="s">
+      <c r="AJ9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -4881,14 +4971,23 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AF10">
+        <v>2</v>
+      </c>
+      <c r="AG10">
+        <v>2</v>
+      </c>
+      <c r="AH10">
+        <v>2</v>
+      </c>
+      <c r="AI10">
         <f>1*3+1*3+1*3+1*3</f>
         <v>12</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AJ10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -4986,14 +5085,23 @@
         <v>1.0099999999999998</v>
       </c>
       <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>2</v>
+      </c>
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AI11">
         <f>1*3+1*3</f>
         <v>6</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AJ11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -5091,14 +5199,23 @@
         <v>0.79999999999999993</v>
       </c>
       <c r="AF12">
+        <v>4</v>
+      </c>
+      <c r="AG12">
+        <v>2</v>
+      </c>
+      <c r="AH12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
         <f>1*3+1*3+1*3+1*3</f>
         <v>12</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AJ12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -5196,14 +5313,23 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AF13">
+        <v>2</v>
+      </c>
+      <c r="AG13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <v>3</v>
+      </c>
+      <c r="AI13">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AJ13" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -5301,14 +5427,23 @@
         <v>1.04</v>
       </c>
       <c r="AF14">
+        <v>3</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14">
+        <v>2</v>
+      </c>
+      <c r="AI14">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AJ14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5406,14 +5541,23 @@
         <v>1.04</v>
       </c>
       <c r="AF15">
+        <v>1</v>
+      </c>
+      <c r="AG15">
+        <v>2</v>
+      </c>
+      <c r="AH15">
+        <v>1</v>
+      </c>
+      <c r="AI15">
         <f>1*3+1*3</f>
         <v>6</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AJ15" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5511,14 +5655,23 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>4</v>
+      </c>
+      <c r="AH16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
         <f>1*3+1*3+1*3+1*3</f>
         <v>12</v>
       </c>
-      <c r="AG16" t="s">
+      <c r="AJ16" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5616,14 +5769,23 @@
         <v>0.99499999999999988</v>
       </c>
       <c r="AF17">
+        <v>2</v>
+      </c>
+      <c r="AG17">
+        <v>2</v>
+      </c>
+      <c r="AH17">
+        <v>1</v>
+      </c>
+      <c r="AI17">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG17" t="s">
+      <c r="AJ17" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -5721,14 +5883,23 @@
         <v>0.93499999999999994</v>
       </c>
       <c r="AF18">
+        <v>3</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>2</v>
+      </c>
+      <c r="AI18">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AJ18" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -5825,15 +5996,24 @@
         <f t="shared" si="1"/>
         <v>1.1749999999999998</v>
       </c>
-      <c r="AF19">
+      <c r="AF19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AI19">
         <f>1*3+1*3</f>
         <v>6</v>
       </c>
-      <c r="AG19" t="s">
+      <c r="AJ19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -5931,14 +6111,23 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AF20">
+        <v>3</v>
+      </c>
+      <c r="AG20">
+        <v>2</v>
+      </c>
+      <c r="AH20">
+        <v>1</v>
+      </c>
+      <c r="AI20">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG20" t="s">
+      <c r="AJ20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -6035,15 +6224,24 @@
         <f t="shared" si="1"/>
         <v>0.99499999999999988</v>
       </c>
-      <c r="AF21">
+      <c r="AF21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG21" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI21">
         <f>1*3+1*2+1*2+1*2+1*2</f>
         <v>11</v>
       </c>
-      <c r="AG21" t="s">
+      <c r="AJ21" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -6141,14 +6339,23 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="AF22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>2</v>
+      </c>
+      <c r="AH22">
+        <v>2</v>
+      </c>
+      <c r="AI22">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG22" t="s">
+      <c r="AJ22" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -6245,15 +6452,24 @@
         <f t="shared" si="1"/>
         <v>0.96499999999999986</v>
       </c>
-      <c r="AF23">
+      <c r="AF23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI23">
         <f>1*3+1*3+1*3</f>
         <v>9</v>
       </c>
-      <c r="AG23" t="s">
+      <c r="AJ23" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -6350,15 +6566,24 @@
         <f t="shared" si="1"/>
         <v>1.325</v>
       </c>
-      <c r="AF24">
+      <c r="AF24" s="2">
+        <v>3</v>
+      </c>
+      <c r="AG24" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH24" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI24">
         <f>1*3+1*3+1*3+1*3+1*2</f>
         <v>14</v>
       </c>
-      <c r="AG24" t="s">
+      <c r="AJ24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -6455,15 +6680,24 @@
         <f t="shared" si="1"/>
         <v>1.2049999999999998</v>
       </c>
-      <c r="AF25">
+      <c r="AF25" s="2">
+        <v>2</v>
+      </c>
+      <c r="AG25" s="2">
+        <v>4</v>
+      </c>
+      <c r="AH25" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI25">
         <f>1*3+1*3+1*3+1*2+1*1</f>
         <v>12</v>
       </c>
-      <c r="AG25" t="s">
+      <c r="AJ25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -6560,15 +6794,24 @@
         <f t="shared" si="1"/>
         <v>1.2349999999999999</v>
       </c>
-      <c r="AF26">
+      <c r="AF26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI26">
         <f>1*3</f>
         <v>3</v>
       </c>
-      <c r="AG26" t="s">
+      <c r="AJ26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
         <v>90</v>
       </c>
@@ -6579,7 +6822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
         <v>61</v>
       </c>
@@ -6590,7 +6833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
         <v>62</v>
       </c>
@@ -6601,7 +6844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
         <v>63</v>
       </c>

</xml_diff>